<commit_message>
refactor(academic-management): update docs, DDL, procedures, and rename evaluation insert script
</commit_message>
<xml_diff>
--- a/academic-management/docs/Normalización.xlsx
+++ b/academic-management/docs/Normalización.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL_3505\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JsLealM\academic-management-system\academic-management-system\academic-management\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A06048-CEC6-486F-A9AB-35D15F5F08D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16815" windowHeight="7650" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coceptualizacion" sheetId="1" r:id="rId1"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>study_2025</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0" shapeId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -118,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -202,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +287,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0">
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -370,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -454,7 +455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B24" authorId="0" shapeId="0">
+    <comment ref="B24" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -538,7 +539,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B28" authorId="0" shapeId="0">
+    <comment ref="B28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -622,7 +623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -706,7 +707,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B32" authorId="0" shapeId="0">
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -790,7 +791,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -874,7 +875,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B36" authorId="0" shapeId="0">
+    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -958,91 +959,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>study_2025:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tabla Base</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">: Tablas principales que almacena lógica del negocio. Ej(Clientes, Productos, Empleados, Cursos).
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tabla Intermedia</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">: Usada en relaciones muchos a muchos (N:M) contiene claves foráneas de otras tablas. Ej(Estudiantes_Cursos, ProductoPedido, AvionesAerolinea).
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Tablas de Referencia</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">: Contienen valores fijos y estáticos que se usan como listas o catalogos. Ej (TipoDocumento, Paises, Generos, EstadosCiviles).
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B40" authorId="0" shapeId="0">
+    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1131,7 +1048,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="122">
   <si>
     <t>NORMALIZACION BASE DE DATOS</t>
   </si>
@@ -1613,9 +1530,6 @@
     <t>ana@uni.edu</t>
   </si>
   <si>
-    <t>activo</t>
-  </si>
-  <si>
     <t>first_name</t>
   </si>
   <si>
@@ -1661,9 +1575,6 @@
     <t>PREREQUISITE</t>
   </si>
   <si>
-    <t>ACADEMIC_PERIOD</t>
-  </si>
-  <si>
     <t>COURSE_ASSIGNMENT</t>
   </si>
   <si>
@@ -1676,48 +1587,24 @@
     <t>2002-05-15</t>
   </si>
   <si>
-    <t>EVALUATION_GRADE</t>
-  </si>
-  <si>
     <t>SCHEDULE</t>
   </si>
   <si>
     <t>CLASSROOM</t>
   </si>
   <si>
-    <t>SYSTEM_USER</t>
-  </si>
-  <si>
-    <t>AUDIT_LOG</t>
-  </si>
-  <si>
     <t>Todos los atributos no clave dependen completamente de la clave primaria</t>
   </si>
   <si>
     <t>No hay dependencias parciales en tablas con claves compuestas</t>
   </si>
   <si>
-    <t>teacher_id</t>
-  </si>
-  <si>
-    <t>degree</t>
-  </si>
-  <si>
-    <t>knowledge_area</t>
-  </si>
-  <si>
     <t>Carlos Pérez</t>
   </si>
   <si>
     <t>c.perez@uni.edu</t>
   </si>
   <si>
-    <t>MSc</t>
-  </si>
-  <si>
-    <t>Matemáticas</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -1725,12 +1612,36 @@
   </si>
   <si>
     <t>Pérez</t>
+  </si>
+  <si>
+    <t>PROFESSOR</t>
+  </si>
+  <si>
+    <t>professor_id</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>PERIOD</t>
+  </si>
+  <si>
+    <t>GRADE_EVALUATION</t>
+  </si>
+  <si>
+    <t>Computer Science</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>SYSTEM_AUDIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1927,7 +1838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1984,6 +1895,9 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1996,8 +1910,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2011,57 +1970,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2169,39 +2080,44 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>393423</xdr:colOff>
+      <xdr:colOff>570291</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>94738</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>415747</xdr:colOff>
+      <xdr:colOff>238879</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>31059</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4834972" y="767700"/>
-          <a:ext cx="7704443" cy="4222571"/>
+          <a:off x="5489673" y="755885"/>
+          <a:ext cx="7579941" cy="4060086"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2214,30 +2130,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TIPO_GENERAL" displayName="TIPO_GENERAL" ref="A1:A33" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:A33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="TIPO_GENERAL" displayName="TIPO_GENERAL" ref="A1:A33" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A1:A33" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="TIPO_GENERAL" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TIPO_GENERAL" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TIPO_ESPECIFICO" displayName="TIPO_ESPECIFICO" ref="B1:B63" totalsRowShown="0" dataDxfId="3">
-  <autoFilter ref="B1:B63"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="TIPO_ESPECIFICO" displayName="TIPO_ESPECIFICO" ref="B1:B63" totalsRowShown="0" dataDxfId="3">
+  <autoFilter ref="B1:B63" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="TIPO_ESPECIFICO" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TIPO_ESPECIFICO" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="TIPO_TABLA" displayName="TIPO_TABLA" ref="C1:C5" totalsRowShown="0" dataDxfId="1">
-  <autoFilter ref="C1:C5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="TIPO_TABLA" displayName="TIPO_TABLA" ref="C1:C5" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="C1:C5" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="TIPO_TABLA" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TIPO_TABLA" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2539,55 +2455,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="7" max="8" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2597,13 +2513,13 @@
       <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+    </row>
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
@@ -2613,13 +2529,13 @@
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>3</v>
       </c>
@@ -2629,13 +2545,13 @@
       <c r="C7" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -2645,13 +2561,13 @@
       <c r="C8" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
@@ -2675,53 +2591,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" zoomScale="68" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="68" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="G3" s="44" t="s">
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="G3" s="35" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
         <v>18</v>
       </c>
@@ -2732,7 +2648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>77</v>
       </c>
@@ -2743,22 +2659,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
       <c r="J7"/>
@@ -2766,7 +2676,7 @@
       <c r="L7"/>
       <c r="M7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="20" t="s">
         <v>18</v>
       </c>
@@ -2776,41 +2686,26 @@
       <c r="C8" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>65</v>
       </c>
       <c r="C9" s="19">
-        <v>6</v>
-      </c>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="45"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B11" s="43"/>
-      <c r="C11" s="43"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>18</v>
       </c>
@@ -2820,12 +2715,10 @@
       <c r="C12" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>65</v>
@@ -2833,26 +2726,15 @@
       <c r="C13" s="19">
         <v>4</v>
       </c>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="20" t="s">
         <v>18</v>
       </c>
@@ -2862,12 +2744,10 @@
       <c r="C16" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="45"/>
-      <c r="E16" s="45"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="19" t="s">
         <v>66</v>
@@ -2875,26 +2755,15 @@
       <c r="C17" s="19">
         <v>2</v>
       </c>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="43" t="s">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="20" t="s">
         <v>18</v>
       </c>
@@ -2904,12 +2773,10 @@
       <c r="C20" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>65</v>
@@ -2917,26 +2784,15 @@
       <c r="C21" s="19">
         <v>4</v>
       </c>
-      <c r="D21" s="45"/>
-      <c r="E21" s="45"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="45"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="43"/>
-      <c r="C23" s="43"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>18</v>
       </c>
@@ -2946,45 +2802,26 @@
       <c r="C24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B25" s="19" t="s">
         <v>67</v>
       </c>
       <c r="C25" s="19">
-        <v>6</v>
-      </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="45"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="43" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>18</v>
       </c>
@@ -2994,16 +2831,15 @@
       <c r="C28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="45"/>
-      <c r="E28" s="43" t="s">
+      <c r="E28" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="19" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B29" s="19" t="s">
         <v>67</v>
@@ -3011,7 +2847,6 @@
       <c r="C29" s="19">
         <v>4</v>
       </c>
-      <c r="D29" s="45"/>
       <c r="E29" s="20" t="s">
         <v>18</v>
       </c>
@@ -3022,13 +2857,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="E30" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F30" s="19" t="s">
         <v>65</v>
@@ -3037,16 +2868,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="20" t="s">
         <v>18</v>
       </c>
@@ -3056,16 +2885,15 @@
       <c r="C32" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="49" t="s">
+      <c r="E32" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="F32" s="49"/>
-      <c r="G32" s="49"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="19" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B33" s="19" t="s">
         <v>65</v>
@@ -3073,7 +2901,6 @@
       <c r="C33" s="19">
         <v>4</v>
       </c>
-      <c r="D33" s="45"/>
       <c r="E33" s="20" t="s">
         <v>18</v>
       </c>
@@ -3084,31 +2911,25 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="45"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="45"/>
-      <c r="D34" s="45"/>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="E34" s="19" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G34" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="43" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="20" t="s">
         <v>18</v>
       </c>
@@ -3118,16 +2939,10 @@
       <c r="C36" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="19" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B37" s="19" t="s">
         <v>66</v>
@@ -3135,41 +2950,15 @@
       <c r="C37" s="19">
         <v>4</v>
       </c>
-      <c r="D37" s="45"/>
-      <c r="E37" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F37" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="45"/>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="G38" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="43" t="s">
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B39" s="43"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="45"/>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>18</v>
       </c>
@@ -3179,14 +2968,10 @@
       <c r="C40" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="19" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B41" s="19" t="s">
         <v>65</v>
@@ -3194,24 +2979,15 @@
       <c r="C41" s="19">
         <v>8</v>
       </c>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="48"/>
-      <c r="C42" s="48"/>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="41" t="s">
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="B43" s="41"/>
-      <c r="C43" s="41"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -3221,21 +2997,21 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="47"/>
-      <c r="B44" s="47"/>
-      <c r="C44" s="47"/>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="33"/>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="26"/>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="28"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="19" t="s">
         <v>78</v>
       </c>
@@ -3252,7 +3028,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>1</v>
       </c>
@@ -3260,119 +3036,96 @@
         <v>83</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D47" s="19" t="s">
         <v>85</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="45"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B49" s="35"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="26"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" s="47"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="47"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="19" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C50" s="19" t="s">
         <v>81</v>
       </c>
       <c r="D50" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="E50" s="19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>10</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="E51" s="19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="45"/>
-      <c r="B52" s="45"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="36" t="s">
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-    </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="37" t="s">
+      <c r="B54" s="31"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+    </row>
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="25" t="s">
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="B57" s="35"/>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="35"/>
-      <c r="G57" s="35"/>
-      <c r="H57" s="26"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="27"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="28"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B58" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C58" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="C58" s="19" t="s">
+      <c r="D58" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="E58" s="19" t="s">
         <v>89</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>90</v>
       </c>
       <c r="F58" s="19" t="s">
         <v>80</v>
@@ -3384,21 +3137,21 @@
         <v>82</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>1</v>
       </c>
       <c r="B59" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C59" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C59" s="19" t="s">
+      <c r="D59" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="E59" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>94</v>
       </c>
       <c r="F59" s="19" t="s">
         <v>84</v>
@@ -3407,64 +3160,65 @@
         <v>85</v>
       </c>
       <c r="H59" s="19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="47"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B62" s="19" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B61" s="35"/>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="26"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B62" s="19" t="s">
-        <v>87</v>
-      </c>
       <c r="C62" s="19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D62" s="19" t="s">
         <v>81</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F62" s="19" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>10</v>
       </c>
       <c r="B63" s="19" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E63" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="F63" s="19" t="s">
-        <v>120</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A23:C23"/>
     <mergeCell ref="A57:H57"/>
-    <mergeCell ref="A61:F61"/>
-    <mergeCell ref="A49:E49"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="A39:C39"/>
@@ -3473,16 +3227,8 @@
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A61:E61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3491,11 +3237,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Listas!$C$2:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>B5 B9 B13 B17 B21 B25 B29 B33 B37 F30 F34 B41 F38 F40</xm:sqref>
+          <xm:sqref>B5 B9 B13 B17 B21 B25 B29 B33 B37 F30 B41 F34 F40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3504,71 +3250,71 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="84" zoomScaleNormal="155" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="31" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A4:E4"/>
@@ -3580,76 +3326,76 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView zoomScale="47" zoomScaleNormal="155" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="46" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:E3"/>
@@ -3661,59 +3407,59 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="155" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
-    <col min="11" max="11" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="46" t="s">
         <v>73</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-    </row>
-    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+    </row>
+    <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -3728,13 +3474,13 @@
       <c r="J6"/>
       <c r="K6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="31.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:E3"/>
@@ -3746,21 +3492,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="310" zoomScaleNormal="310" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -3771,7 +3517,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -3782,7 +3528,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>23</v>
       </c>
@@ -3793,7 +3539,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="18" t="s">
         <v>23</v>
       </c>
@@ -3804,7 +3550,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
@@ -3815,7 +3561,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>23</v>
       </c>
@@ -3824,7 +3570,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>23</v>
       </c>
@@ -3833,7 +3579,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>23</v>
       </c>
@@ -3842,7 +3588,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>23</v>
       </c>
@@ -3851,7 +3597,7 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>23</v>
       </c>
@@ -3860,7 +3606,7 @@
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>23</v>
       </c>
@@ -3869,7 +3615,7 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="18" t="s">
         <v>33</v>
       </c>
@@ -3878,7 +3624,7 @@
       </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="17" t="s">
         <v>33</v>
       </c>
@@ -3887,7 +3633,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="18" t="s">
         <v>33</v>
       </c>
@@ -3896,7 +3642,7 @@
       </c>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="17" t="s">
         <v>37</v>
       </c>
@@ -3905,7 +3651,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="18" t="s">
         <v>37</v>
       </c>
@@ -3914,7 +3660,7 @@
       </c>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="17" t="s">
         <v>37</v>
       </c>
@@ -3923,7 +3669,7 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="18" t="s">
         <v>37</v>
       </c>
@@ -3932,7 +3678,7 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>42</v>
       </c>
@@ -3941,7 +3687,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="18" t="s">
         <v>44</v>
       </c>
@@ -3950,7 +3696,7 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>46</v>
       </c>
@@ -3959,7 +3705,7 @@
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="18" t="s">
         <v>47</v>
       </c>
@@ -3968,7 +3714,7 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="17" t="s">
         <v>47</v>
       </c>
@@ -3977,7 +3723,7 @@
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="18" t="s">
         <v>47</v>
       </c>
@@ -3986,7 +3732,7 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="17" t="s">
         <v>51</v>
       </c>
@@ -3995,7 +3741,7 @@
       </c>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>53</v>
       </c>
@@ -4004,7 +3750,7 @@
       </c>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="17" t="s">
         <v>53</v>
       </c>
@@ -4013,7 +3759,7 @@
       </c>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
         <v>56</v>
       </c>
@@ -4022,7 +3768,7 @@
       </c>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="17" t="s">
         <v>58</v>
       </c>
@@ -4031,7 +3777,7 @@
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
         <v>58</v>
       </c>
@@ -4040,7 +3786,7 @@
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
         <v>58</v>
       </c>
@@ -4049,7 +3795,7 @@
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
         <v>58</v>
       </c>
@@ -4058,7 +3804,7 @@
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="17" t="s">
         <v>58</v>
       </c>
@@ -4067,123 +3813,123 @@
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
@@ -4198,6 +3944,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c75b117b-0cac-4216-91ce-aec485cc8c94">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="416e0ee7-af69-444a-bf3e-43ee4c281f82" xsi:nil="true"/>
+    <ReferenceId xmlns="c75b117b-0cac-4216-91ce-aec485cc8c94" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AE01B0DCCB2664469966EB4707D3D0D4" ma:contentTypeVersion="12" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="7eaf2bfe837720a2d1bb357f378c1b4b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c75b117b-0cac-4216-91ce-aec485cc8c94" xmlns:ns3="416e0ee7-af69-444a-bf3e-43ee4c281f82" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d70b6a921727c74ad3c2ba4a7174d1a1" ns2:_="" ns3:_="">
     <xsd:import namespace="c75b117b-0cac-4216-91ce-aec485cc8c94"/>
@@ -4398,28 +4165,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c75b117b-0cac-4216-91ce-aec485cc8c94">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="416e0ee7-af69-444a-bf3e-43ee4c281f82" xsi:nil="true"/>
-    <ReferenceId xmlns="c75b117b-0cac-4216-91ce-aec485cc8c94" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B25E826B-C44E-43A0-A077-EBC78B087884}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3E99EA-2CC2-47FF-9659-2C7B5845CC53}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c75b117b-0cac-4216-91ce-aec485cc8c94"/>
+    <ds:schemaRef ds:uri="416e0ee7-af69-444a-bf3e-43ee4c281f82"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D5A117CF-5CCC-4FC4-A723-1696EFB2AB06}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4436,23 +4201,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E3E99EA-2CC2-47FF-9659-2C7B5845CC53}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c75b117b-0cac-4216-91ce-aec485cc8c94"/>
-    <ds:schemaRef ds:uri="416e0ee7-af69-444a-bf3e-43ee4c281f82"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B25E826B-C44E-43A0-A077-EBC78B087884}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>